<commit_message>
geting the final polished version of the R tutorial
</commit_message>
<xml_diff>
--- a/R/data_files/snark.measures.xlsx
+++ b/R/data_files/snark.measures.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="41">
   <si>
     <t>We're still waiting on the TDF pop, but this is the measurements for the snarks that we have. We measured length and width of the armor plated cephalocalypsis from a photograph using calipers and a sextant. The units are millimeters.</t>
   </si>
@@ -126,7 +126,13 @@
     <t>8.0236794112*</t>
   </si>
   <si>
+    <t>6.01613987474441*</t>
+  </si>
+  <si>
     <t>Juneau</t>
+  </si>
+  <si>
+    <t>388.26000185323*</t>
   </si>
   <si>
     <t>35.6865474280811*</t>
@@ -391,7 +397,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -416,8 +422,8 @@
       <c:layout/>
     </c:title>
     <c:view3D>
-      <c:rotX val="16"/>
-      <c:rotY val="21"/>
+      <c:rotX val="17"/>
+      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
       <c:perspective val="40"/>
     </c:view3D>
@@ -546,14 +552,24 @@
             </a:ln>
           </c:spPr>
         </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="cylinder"/>
-        <c:axId val="26489011"/>
-        <c:axId val="32722288"/>
+        <c:axId val="13863742"/>
+        <c:axId val="46439789"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="26489011"/>
+        <c:axId val="13863742"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,14 +585,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="32722288"/>
+        <c:crossAx val="46439789"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32722288"/>
+        <c:axId val="46439789"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,7 +617,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26489011"/>
+        <c:crossAx val="13863742"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -641,15 +657,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>181440</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:colOff>208440</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>249840</xdr:colOff>
+      <xdr:colOff>276480</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -657,8 +673,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5870880" y="1138320"/>
-        <a:ext cx="5757840" cy="3237840"/>
+        <a:off x="5897880" y="1129320"/>
+        <a:ext cx="5757480" cy="3237480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -678,8 +694,8 @@
   </sheetPr>
   <dimension ref="A1:AC982"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W7" activeCellId="0" sqref="W7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N541" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O556" activeCellId="0" sqref="O556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -21249,8 +21265,8 @@
       <c r="F295" s="6" t="n">
         <v>0.606676923266667</v>
       </c>
-      <c r="G295" s="6" t="n">
-        <v>6.01613987474441</v>
+      <c r="G295" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="H295" s="6" t="n">
         <v>2.94706397066667</v>
@@ -22794,7 +22810,7 @@
     </row>
     <row r="317" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B317" s="7" t="n">
         <v>0</v>
@@ -22886,7 +22902,7 @@
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B318" s="7" t="n">
         <v>0</v>
@@ -22957,7 +22973,7 @@
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B319" s="7" t="n">
         <v>0</v>
@@ -23028,7 +23044,7 @@
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B320" s="7" t="n">
         <v>0</v>
@@ -23099,7 +23115,7 @@
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B321" s="7" t="n">
         <v>0</v>
@@ -23170,7 +23186,7 @@
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B322" s="7" t="n">
         <v>0</v>
@@ -23241,7 +23257,7 @@
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B323" s="7" t="n">
         <v>0</v>
@@ -23312,7 +23328,7 @@
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B324" s="7" t="n">
         <v>0</v>
@@ -23383,7 +23399,7 @@
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B325" s="7" t="n">
         <v>0</v>
@@ -23454,7 +23470,7 @@
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B326" s="7" t="n">
         <v>0</v>
@@ -23525,7 +23541,7 @@
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B327" s="7" t="n">
         <v>0</v>
@@ -23596,7 +23612,7 @@
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B328" s="7" t="n">
         <v>0</v>
@@ -23667,7 +23683,7 @@
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B329" s="7" t="n">
         <v>0</v>
@@ -23738,7 +23754,7 @@
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B330" s="7" t="n">
         <v>0</v>
@@ -23809,7 +23825,7 @@
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B331" s="7" t="n">
         <v>0</v>
@@ -23880,7 +23896,7 @@
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B332" s="7" t="n">
         <v>0</v>
@@ -23951,7 +23967,7 @@
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B333" s="7" t="n">
         <v>0</v>
@@ -24022,7 +24038,7 @@
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B334" s="7" t="n">
         <v>0</v>
@@ -24093,7 +24109,7 @@
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B335" s="7" t="n">
         <v>0</v>
@@ -24164,7 +24180,7 @@
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B336" s="7" t="n">
         <v>0</v>
@@ -24235,7 +24251,7 @@
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B337" s="7" t="n">
         <v>0</v>
@@ -24306,7 +24322,7 @@
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B338" s="7" t="n">
         <v>0</v>
@@ -24377,7 +24393,7 @@
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B339" s="7" t="n">
         <v>0</v>
@@ -24448,7 +24464,7 @@
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B340" s="7" t="n">
         <v>0</v>
@@ -24519,7 +24535,7 @@
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B341" s="7" t="n">
         <v>0</v>
@@ -24590,7 +24606,7 @@
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B342" s="7" t="n">
         <v>0</v>
@@ -24661,7 +24677,7 @@
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B343" s="7" t="n">
         <v>0</v>
@@ -24732,7 +24748,7 @@
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B344" s="7" t="n">
         <v>0</v>
@@ -24803,7 +24819,7 @@
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B345" s="7" t="n">
         <v>0</v>
@@ -24874,7 +24890,7 @@
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B346" s="7" t="n">
         <v>0</v>
@@ -24945,7 +24961,7 @@
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B347" s="7" t="n">
         <v>0</v>
@@ -25016,7 +25032,7 @@
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B348" s="7" t="n">
         <v>0</v>
@@ -25087,7 +25103,7 @@
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B349" s="7" t="n">
         <v>0</v>
@@ -25158,7 +25174,7 @@
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B350" s="7" t="n">
         <v>0</v>
@@ -25229,7 +25245,7 @@
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B351" s="7" t="n">
         <v>0</v>
@@ -25300,7 +25316,7 @@
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B352" s="7" t="n">
         <v>0</v>
@@ -25371,7 +25387,7 @@
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B353" s="7" t="n">
         <v>0</v>
@@ -25442,7 +25458,7 @@
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B354" s="7" t="n">
         <v>0</v>
@@ -25513,7 +25529,7 @@
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B355" s="7" t="n">
         <v>0</v>
@@ -25584,7 +25600,7 @@
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B356" s="7" t="n">
         <v>0</v>
@@ -25655,7 +25671,7 @@
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B357" s="7" t="n">
         <v>0</v>
@@ -25726,7 +25742,7 @@
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B358" s="7" t="n">
         <v>0</v>
@@ -25797,7 +25813,7 @@
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B359" s="7" t="n">
         <v>0</v>
@@ -25868,7 +25884,7 @@
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B360" s="7" t="n">
         <v>0</v>
@@ -25939,7 +25955,7 @@
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B361" s="7" t="n">
         <v>0</v>
@@ -26010,7 +26026,7 @@
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B362" s="7" t="n">
         <v>0</v>
@@ -26081,7 +26097,7 @@
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B363" s="7" t="n">
         <v>0</v>
@@ -26152,7 +26168,7 @@
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B364" s="7" t="n">
         <v>0</v>
@@ -26223,7 +26239,7 @@
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B365" s="7" t="n">
         <v>0</v>
@@ -26294,7 +26310,7 @@
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B366" s="7" t="n">
         <v>0</v>
@@ -26365,7 +26381,7 @@
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B367" s="7" t="n">
         <v>0</v>
@@ -26436,7 +26452,7 @@
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B368" s="7" t="n">
         <v>0</v>
@@ -26507,7 +26523,7 @@
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B369" s="7" t="n">
         <v>0</v>
@@ -26578,7 +26594,7 @@
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B370" s="7" t="n">
         <v>0</v>
@@ -26649,7 +26665,7 @@
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B371" s="7" t="n">
         <v>0</v>
@@ -26720,7 +26736,7 @@
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B372" s="7" t="n">
         <v>0</v>
@@ -26791,7 +26807,7 @@
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B373" s="7" t="n">
         <v>0</v>
@@ -26862,7 +26878,7 @@
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B374" s="7" t="n">
         <v>0</v>
@@ -26933,7 +26949,7 @@
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B375" s="7" t="n">
         <v>0</v>
@@ -27004,7 +27020,7 @@
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B376" s="7" t="n">
         <v>0</v>
@@ -27075,7 +27091,7 @@
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B377" s="7" t="n">
         <v>0</v>
@@ -27146,7 +27162,7 @@
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B378" s="7" t="n">
         <v>0</v>
@@ -27217,7 +27233,7 @@
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B379" s="7" t="n">
         <v>0</v>
@@ -27288,7 +27304,7 @@
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B380" s="7" t="n">
         <v>0</v>
@@ -27359,7 +27375,7 @@
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B381" s="7" t="n">
         <v>0</v>
@@ -27430,7 +27446,7 @@
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B382" s="7" t="n">
         <v>0</v>
@@ -27501,7 +27517,7 @@
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B383" s="7" t="n">
         <v>0</v>
@@ -27572,7 +27588,7 @@
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B384" s="7" t="n">
         <v>0</v>
@@ -27643,7 +27659,7 @@
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B385" s="7" t="n">
         <v>0</v>
@@ -27714,7 +27730,7 @@
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B386" s="7" t="n">
         <v>0</v>
@@ -27785,7 +27801,7 @@
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B387" s="7" t="n">
         <v>0</v>
@@ -27856,7 +27872,7 @@
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B388" s="7" t="n">
         <v>0</v>
@@ -27927,7 +27943,7 @@
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B389" s="7" t="n">
         <v>0</v>
@@ -27998,7 +28014,7 @@
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B390" s="7" t="n">
         <v>0</v>
@@ -28069,7 +28085,7 @@
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B391" s="7" t="n">
         <v>0</v>
@@ -28140,7 +28156,7 @@
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B392" s="7" t="n">
         <v>0</v>
@@ -28211,7 +28227,7 @@
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B393" s="7" t="n">
         <v>0</v>
@@ -28282,7 +28298,7 @@
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B394" s="7" t="n">
         <v>0</v>
@@ -28353,7 +28369,7 @@
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B395" s="7" t="n">
         <v>0</v>
@@ -28424,7 +28440,7 @@
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B396" s="7" t="n">
         <v>0</v>
@@ -28495,7 +28511,7 @@
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B397" s="7" t="n">
         <v>0</v>
@@ -28566,7 +28582,7 @@
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B398" s="7" t="n">
         <v>0</v>
@@ -28637,7 +28653,7 @@
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B399" s="7" t="n">
         <v>0</v>
@@ -28708,7 +28724,7 @@
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B400" s="7" t="n">
         <v>0</v>
@@ -28779,7 +28795,7 @@
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B401" s="7" t="n">
         <v>0</v>
@@ -28850,7 +28866,7 @@
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B402" s="7" t="n">
         <v>0</v>
@@ -28921,7 +28937,7 @@
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B403" s="7" t="n">
         <v>0</v>
@@ -28992,7 +29008,7 @@
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B404" s="7" t="n">
         <v>0</v>
@@ -29063,7 +29079,7 @@
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B405" s="7" t="n">
         <v>0</v>
@@ -29134,7 +29150,7 @@
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B406" s="7" t="n">
         <v>0</v>
@@ -29205,7 +29221,7 @@
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B407" s="7" t="n">
         <v>0</v>
@@ -29276,7 +29292,7 @@
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B408" s="7" t="n">
         <v>0</v>
@@ -29347,7 +29363,7 @@
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B409" s="7" t="n">
         <v>0</v>
@@ -29418,7 +29434,7 @@
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B410" s="7" t="n">
         <v>0</v>
@@ -29489,7 +29505,7 @@
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B411" s="7" t="n">
         <v>0</v>
@@ -29560,7 +29576,7 @@
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B412" s="7" t="n">
         <v>0</v>
@@ -29631,7 +29647,7 @@
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B413" s="7" t="n">
         <v>0</v>
@@ -29702,7 +29718,7 @@
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B414" s="7" t="n">
         <v>0</v>
@@ -29773,7 +29789,7 @@
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B415" s="7" t="n">
         <v>0</v>
@@ -29844,7 +29860,7 @@
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B416" s="7" t="n">
         <v>0</v>
@@ -29915,7 +29931,7 @@
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B417" s="7" t="n">
         <v>0</v>
@@ -29986,7 +30002,7 @@
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B418" s="7" t="n">
         <v>0</v>
@@ -30057,7 +30073,7 @@
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B419" s="7" t="n">
         <v>0</v>
@@ -30128,7 +30144,7 @@
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B420" s="7" t="n">
         <v>0</v>
@@ -30199,7 +30215,7 @@
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B421" s="7" t="n">
         <v>0</v>
@@ -30270,7 +30286,7 @@
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B422" s="7" t="n">
         <v>0</v>
@@ -30341,7 +30357,7 @@
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B423" s="7" t="n">
         <v>0</v>
@@ -30412,7 +30428,7 @@
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B424" s="7" t="n">
         <v>0</v>
@@ -30483,7 +30499,7 @@
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B425" s="7" t="n">
         <v>0</v>
@@ -30554,7 +30570,7 @@
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B426" s="7" t="n">
         <v>0</v>
@@ -30625,7 +30641,7 @@
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B427" s="7" t="n">
         <v>0</v>
@@ -30696,7 +30712,7 @@
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B428" s="7" t="n">
         <v>0</v>
@@ -30767,7 +30783,7 @@
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B429" s="7" t="n">
         <v>0</v>
@@ -30838,7 +30854,7 @@
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B430" s="7" t="n">
         <v>0</v>
@@ -30909,7 +30925,7 @@
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B431" s="7" t="n">
         <v>0</v>
@@ -30980,7 +30996,7 @@
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B432" s="7" t="n">
         <v>0</v>
@@ -31051,7 +31067,7 @@
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B433" s="7" t="n">
         <v>0</v>
@@ -31122,7 +31138,7 @@
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B434" s="7" t="n">
         <v>0</v>
@@ -31193,7 +31209,7 @@
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B435" s="7" t="n">
         <v>0</v>
@@ -31264,7 +31280,7 @@
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B436" s="7" t="n">
         <v>0</v>
@@ -31335,7 +31351,7 @@
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B437" s="7" t="n">
         <v>0</v>
@@ -31406,7 +31422,7 @@
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B438" s="7" t="n">
         <v>0</v>
@@ -31477,7 +31493,7 @@
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B439" s="7" t="n">
         <v>0</v>
@@ -31548,7 +31564,7 @@
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B440" s="7" t="n">
         <v>0</v>
@@ -31619,7 +31635,7 @@
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B441" s="7" t="n">
         <v>0</v>
@@ -31690,7 +31706,7 @@
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B442" s="7" t="n">
         <v>0</v>
@@ -31761,7 +31777,7 @@
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B443" s="7" t="n">
         <v>0</v>
@@ -31832,7 +31848,7 @@
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B444" s="7" t="n">
         <v>0</v>
@@ -31903,7 +31919,7 @@
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B445" s="7" t="n">
         <v>0</v>
@@ -31974,7 +31990,7 @@
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B446" s="7" t="n">
         <v>0</v>
@@ -32045,7 +32061,7 @@
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B447" s="7" t="n">
         <v>0</v>
@@ -32116,7 +32132,7 @@
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B448" s="7" t="n">
         <v>0</v>
@@ -32187,7 +32203,7 @@
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B449" s="7" t="n">
         <v>0</v>
@@ -32258,7 +32274,7 @@
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B450" s="7" t="n">
         <v>0</v>
@@ -32329,7 +32345,7 @@
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B451" s="7" t="n">
         <v>0</v>
@@ -32400,7 +32416,7 @@
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B452" s="7" t="n">
         <v>0</v>
@@ -32471,7 +32487,7 @@
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B453" s="7" t="n">
         <v>0</v>
@@ -32542,7 +32558,7 @@
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B454" s="7" t="n">
         <v>0</v>
@@ -32613,7 +32629,7 @@
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B455" s="7" t="n">
         <v>0</v>
@@ -32684,7 +32700,7 @@
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B456" s="7" t="n">
         <v>0</v>
@@ -32755,7 +32771,7 @@
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B457" s="7" t="n">
         <v>0</v>
@@ -32826,7 +32842,7 @@
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B458" s="7" t="n">
         <v>0</v>
@@ -32897,7 +32913,7 @@
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B459" s="7" t="n">
         <v>0</v>
@@ -32968,7 +32984,7 @@
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B460" s="7" t="n">
         <v>0</v>
@@ -33039,7 +33055,7 @@
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B461" s="7" t="n">
         <v>0</v>
@@ -33110,7 +33126,7 @@
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B462" s="7" t="n">
         <v>0</v>
@@ -33181,7 +33197,7 @@
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B463" s="7" t="n">
         <v>0</v>
@@ -33252,7 +33268,7 @@
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B464" s="7" t="n">
         <v>0</v>
@@ -33323,7 +33339,7 @@
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B465" s="7" t="n">
         <v>0</v>
@@ -33394,7 +33410,7 @@
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B466" s="7" t="n">
         <v>0</v>
@@ -33465,7 +33481,7 @@
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B467" s="7" t="n">
         <v>0</v>
@@ -33536,7 +33552,7 @@
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B468" s="7" t="n">
         <v>0</v>
@@ -33607,7 +33623,7 @@
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B469" s="7" t="n">
         <v>0</v>
@@ -33678,7 +33694,7 @@
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B470" s="7" t="n">
         <v>0</v>
@@ -33749,7 +33765,7 @@
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B471" s="7" t="n">
         <v>0</v>
@@ -33820,7 +33836,7 @@
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B472" s="7" t="n">
         <v>0</v>
@@ -33891,7 +33907,7 @@
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B473" s="7" t="n">
         <v>0</v>
@@ -33962,7 +33978,7 @@
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B474" s="7" t="n">
         <v>0</v>
@@ -34033,7 +34049,7 @@
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B475" s="7" t="n">
         <v>0</v>
@@ -34104,7 +34120,7 @@
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B476" s="7" t="n">
         <v>0</v>
@@ -34175,7 +34191,7 @@
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B477" s="7" t="n">
         <v>0</v>
@@ -34246,7 +34262,7 @@
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B478" s="7" t="n">
         <v>0</v>
@@ -34317,7 +34333,7 @@
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B479" s="7" t="n">
         <v>0</v>
@@ -34388,7 +34404,7 @@
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B480" s="7" t="n">
         <v>0</v>
@@ -34459,7 +34475,7 @@
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B481" s="7" t="n">
         <v>0</v>
@@ -34530,7 +34546,7 @@
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B482" s="7" t="n">
         <v>0</v>
@@ -34601,7 +34617,7 @@
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B483" s="7" t="n">
         <v>0</v>
@@ -34672,7 +34688,7 @@
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B484" s="7" t="n">
         <v>0</v>
@@ -34743,7 +34759,7 @@
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B485" s="7" t="n">
         <v>0</v>
@@ -34814,7 +34830,7 @@
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B486" s="7" t="n">
         <v>0</v>
@@ -34885,7 +34901,7 @@
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B487" s="7" t="n">
         <v>0</v>
@@ -34956,7 +34972,7 @@
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B488" s="7" t="n">
         <v>0</v>
@@ -35027,7 +35043,7 @@
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B489" s="7" t="n">
         <v>0</v>
@@ -35098,7 +35114,7 @@
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B490" s="7" t="n">
         <v>0</v>
@@ -35169,7 +35185,7 @@
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B491" s="7" t="n">
         <v>0</v>
@@ -35240,7 +35256,7 @@
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B492" s="7" t="n">
         <v>0</v>
@@ -35311,7 +35327,7 @@
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B493" s="7" t="n">
         <v>0</v>
@@ -35382,7 +35398,7 @@
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B494" s="7" t="n">
         <v>0</v>
@@ -35453,7 +35469,7 @@
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B495" s="7" t="n">
         <v>0</v>
@@ -35524,7 +35540,7 @@
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B496" s="7" t="n">
         <v>0</v>
@@ -35595,7 +35611,7 @@
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B497" s="7" t="n">
         <v>0</v>
@@ -35666,7 +35682,7 @@
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B498" s="7" t="n">
         <v>0</v>
@@ -35737,7 +35753,7 @@
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B499" s="7" t="n">
         <v>0</v>
@@ -35808,7 +35824,7 @@
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B500" s="7" t="n">
         <v>0</v>
@@ -35879,7 +35895,7 @@
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B501" s="7" t="n">
         <v>0</v>
@@ -35950,7 +35966,7 @@
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B502" s="7" t="n">
         <v>0</v>
@@ -36021,7 +36037,7 @@
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B503" s="7" t="n">
         <v>0</v>
@@ -36092,7 +36108,7 @@
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B504" s="7" t="n">
         <v>0</v>
@@ -36163,7 +36179,7 @@
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B505" s="7" t="n">
         <v>0</v>
@@ -36234,7 +36250,7 @@
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B506" s="7" t="n">
         <v>0</v>
@@ -36305,7 +36321,7 @@
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B507" s="7" t="n">
         <v>0</v>
@@ -36376,7 +36392,7 @@
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B508" s="7" t="n">
         <v>0</v>
@@ -36447,7 +36463,7 @@
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B509" s="7" t="n">
         <v>0</v>
@@ -36518,7 +36534,7 @@
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B510" s="7" t="n">
         <v>0</v>
@@ -36589,7 +36605,7 @@
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B511" s="7" t="n">
         <v>0</v>
@@ -36660,7 +36676,7 @@
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B512" s="7" t="n">
         <v>0</v>
@@ -36731,7 +36747,7 @@
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B513" s="7" t="n">
         <v>0</v>
@@ -36802,7 +36818,7 @@
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B514" s="7" t="n">
         <v>0</v>
@@ -36873,7 +36889,7 @@
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B515" s="7" t="n">
         <v>0</v>
@@ -36944,7 +36960,7 @@
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B516" s="7" t="n">
         <v>0</v>
@@ -37015,7 +37031,7 @@
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B517" s="7" t="n">
         <v>0</v>
@@ -37086,7 +37102,7 @@
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B518" s="7" t="n">
         <v>0</v>
@@ -37157,7 +37173,7 @@
     </row>
     <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B519" s="7" t="n">
         <v>0</v>
@@ -37228,7 +37244,7 @@
     </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B520" s="7" t="n">
         <v>0</v>
@@ -37299,7 +37315,7 @@
     </row>
     <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B521" s="7" t="n">
         <v>0</v>
@@ -37370,7 +37386,7 @@
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B522" s="7" t="n">
         <v>0</v>
@@ -37441,7 +37457,7 @@
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B523" s="7" t="n">
         <v>0</v>
@@ -37512,7 +37528,7 @@
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B524" s="7" t="n">
         <v>0</v>
@@ -37583,7 +37599,7 @@
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B525" s="7" t="n">
         <v>0</v>
@@ -37654,7 +37670,7 @@
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B526" s="7" t="n">
         <v>0</v>
@@ -37725,7 +37741,7 @@
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B527" s="7" t="n">
         <v>0</v>
@@ -37796,7 +37812,7 @@
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B528" s="7" t="n">
         <v>0</v>
@@ -37867,7 +37883,7 @@
     </row>
     <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B529" s="7" t="n">
         <v>0</v>
@@ -37938,7 +37954,7 @@
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B530" s="7" t="n">
         <v>0</v>
@@ -38009,7 +38025,7 @@
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B531" s="7" t="n">
         <v>0</v>
@@ -38080,7 +38096,7 @@
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B532" s="7" t="n">
         <v>0</v>
@@ -38151,7 +38167,7 @@
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B533" s="7" t="n">
         <v>0</v>
@@ -38222,7 +38238,7 @@
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B534" s="7" t="n">
         <v>0</v>
@@ -38293,7 +38309,7 @@
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B535" s="7" t="n">
         <v>0</v>
@@ -38364,7 +38380,7 @@
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B536" s="7" t="n">
         <v>0</v>
@@ -38435,7 +38451,7 @@
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B537" s="7" t="n">
         <v>0</v>
@@ -38506,7 +38522,7 @@
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B538" s="7" t="n">
         <v>0</v>
@@ -38577,7 +38593,7 @@
     </row>
     <row r="539" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B539" s="7" t="n">
         <v>0</v>
@@ -38669,7 +38685,7 @@
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B540" s="7" t="n">
         <v>0</v>
@@ -38740,7 +38756,7 @@
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B541" s="7" t="n">
         <v>0</v>
@@ -38811,7 +38827,7 @@
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B542" s="7" t="n">
         <v>0</v>
@@ -38882,7 +38898,7 @@
     </row>
     <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B543" s="7" t="n">
         <v>0</v>
@@ -38953,7 +38969,7 @@
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B544" s="7" t="n">
         <v>0</v>
@@ -39024,7 +39040,7 @@
     </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B545" s="7" t="n">
         <v>0</v>
@@ -39095,7 +39111,7 @@
     </row>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B546" s="10" t="n">
         <v>1</v>
@@ -39166,7 +39182,7 @@
     </row>
     <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B547" s="10" t="n">
         <v>1</v>
@@ -39237,7 +39253,7 @@
     </row>
     <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B548" s="10" t="n">
         <v>1</v>
@@ -39308,7 +39324,7 @@
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B549" s="10" t="n">
         <v>1</v>
@@ -39379,7 +39395,7 @@
     </row>
     <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B550" s="10" t="n">
         <v>1</v>
@@ -39450,7 +39466,7 @@
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B551" s="10" t="n">
         <v>1</v>
@@ -39521,7 +39537,7 @@
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B552" s="10" t="n">
         <v>1</v>
@@ -39592,7 +39608,7 @@
     </row>
     <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B553" s="10" t="n">
         <v>1</v>
@@ -39663,7 +39679,7 @@
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B554" s="10" t="n">
         <v>1</v>
@@ -39734,7 +39750,7 @@
     </row>
     <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B555" s="10" t="n">
         <v>1</v>
@@ -39805,7 +39821,7 @@
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B556" s="10" t="n">
         <v>1</v>
@@ -39846,8 +39862,8 @@
       <c r="N556" s="10" t="n">
         <v>28.1977773594</v>
       </c>
-      <c r="O556" s="10" t="n">
-        <v>388.26000185323</v>
+      <c r="O556" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="P556" s="10" t="n">
         <v>19.92213474075</v>
@@ -39876,7 +39892,7 @@
     </row>
     <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B557" s="10" t="n">
         <v>1</v>
@@ -39947,7 +39963,7 @@
     </row>
     <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B558" s="10" t="n">
         <v>1</v>
@@ -40018,7 +40034,7 @@
     </row>
     <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B559" s="10" t="n">
         <v>1</v>
@@ -40089,7 +40105,7 @@
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B560" s="10" t="n">
         <v>1</v>
@@ -40160,7 +40176,7 @@
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B561" s="10" t="n">
         <v>1</v>
@@ -40231,7 +40247,7 @@
     </row>
     <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B562" s="10" t="n">
         <v>1</v>
@@ -40302,7 +40318,7 @@
     </row>
     <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B563" s="10" t="n">
         <v>1</v>
@@ -40373,7 +40389,7 @@
     </row>
     <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B564" s="10" t="n">
         <v>1</v>
@@ -40444,7 +40460,7 @@
     </row>
     <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B565" s="10" t="n">
         <v>1</v>
@@ -40515,7 +40531,7 @@
     </row>
     <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B566" s="10" t="n">
         <v>1</v>
@@ -40586,7 +40602,7 @@
     </row>
     <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B567" s="10" t="n">
         <v>1</v>
@@ -40657,7 +40673,7 @@
     </row>
     <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B568" s="10" t="n">
         <v>1</v>
@@ -40728,7 +40744,7 @@
     </row>
     <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B569" s="10" t="n">
         <v>1</v>
@@ -40799,7 +40815,7 @@
     </row>
     <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B570" s="10" t="n">
         <v>1</v>
@@ -40870,7 +40886,7 @@
     </row>
     <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B571" s="10" t="n">
         <v>1</v>
@@ -40941,7 +40957,7 @@
     </row>
     <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B572" s="10" t="n">
         <v>1</v>
@@ -41012,7 +41028,7 @@
     </row>
     <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B573" s="10" t="n">
         <v>1</v>
@@ -41083,7 +41099,7 @@
     </row>
     <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B574" s="10" t="n">
         <v>1</v>
@@ -41154,7 +41170,7 @@
     </row>
     <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B575" s="10" t="n">
         <v>1</v>
@@ -41225,7 +41241,7 @@
     </row>
     <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B576" s="10" t="n">
         <v>1</v>
@@ -41296,7 +41312,7 @@
     </row>
     <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B577" s="10" t="n">
         <v>1</v>
@@ -41367,7 +41383,7 @@
     </row>
     <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B578" s="10" t="n">
         <v>1</v>
@@ -41438,7 +41454,7 @@
     </row>
     <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B579" s="10" t="n">
         <v>1</v>
@@ -41509,7 +41525,7 @@
     </row>
     <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B580" s="10" t="n">
         <v>1</v>
@@ -41580,7 +41596,7 @@
     </row>
     <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B581" s="10" t="n">
         <v>1</v>
@@ -41651,7 +41667,7 @@
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B582" s="10" t="n">
         <v>1</v>
@@ -41722,7 +41738,7 @@
     </row>
     <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B583" s="10" t="n">
         <v>1</v>
@@ -41793,7 +41809,7 @@
     </row>
     <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B584" s="10" t="n">
         <v>1</v>
@@ -41864,7 +41880,7 @@
     </row>
     <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B585" s="10" t="n">
         <v>1</v>
@@ -41935,7 +41951,7 @@
     </row>
     <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B586" s="10" t="n">
         <v>1</v>
@@ -42006,7 +42022,7 @@
     </row>
     <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B587" s="10" t="n">
         <v>1</v>
@@ -42077,7 +42093,7 @@
     </row>
     <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B588" s="10" t="n">
         <v>1</v>
@@ -42148,7 +42164,7 @@
     </row>
     <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B589" s="10" t="n">
         <v>1</v>
@@ -42219,7 +42235,7 @@
     </row>
     <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B590" s="10" t="n">
         <v>1</v>
@@ -42290,7 +42306,7 @@
     </row>
     <row r="591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B591" s="10" t="n">
         <v>1</v>
@@ -42361,7 +42377,7 @@
     </row>
     <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B592" s="10" t="n">
         <v>1</v>
@@ -42432,7 +42448,7 @@
     </row>
     <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B593" s="10" t="n">
         <v>1</v>
@@ -42503,7 +42519,7 @@
     </row>
     <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B594" s="10" t="n">
         <v>1</v>
@@ -42574,7 +42590,7 @@
     </row>
     <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B595" s="10" t="n">
         <v>1</v>
@@ -42645,7 +42661,7 @@
     </row>
     <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B596" s="10" t="n">
         <v>1</v>
@@ -42716,7 +42732,7 @@
     </row>
     <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B597" s="10" t="n">
         <v>1</v>
@@ -42787,7 +42803,7 @@
     </row>
     <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B598" s="10" t="n">
         <v>1</v>
@@ -42858,7 +42874,7 @@
     </row>
     <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B599" s="10" t="n">
         <v>1</v>
@@ -42929,7 +42945,7 @@
     </row>
     <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B600" s="10" t="n">
         <v>1</v>
@@ -43000,7 +43016,7 @@
     </row>
     <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B601" s="10" t="n">
         <v>1</v>
@@ -43071,7 +43087,7 @@
     </row>
     <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B602" s="10" t="n">
         <v>1</v>
@@ -43142,7 +43158,7 @@
     </row>
     <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B603" s="10" t="n">
         <v>1</v>
@@ -43213,7 +43229,7 @@
     </row>
     <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B604" s="10" t="n">
         <v>1</v>
@@ -43284,7 +43300,7 @@
     </row>
     <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B605" s="10" t="n">
         <v>1</v>
@@ -43355,7 +43371,7 @@
     </row>
     <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B606" s="10" t="n">
         <v>1</v>
@@ -43426,7 +43442,7 @@
     </row>
     <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B607" s="10" t="n">
         <v>1</v>
@@ -43497,7 +43513,7 @@
     </row>
     <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B608" s="10" t="n">
         <v>1</v>
@@ -43568,7 +43584,7 @@
     </row>
     <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B609" s="10" t="n">
         <v>1</v>
@@ -43639,7 +43655,7 @@
     </row>
     <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B610" s="10" t="n">
         <v>1</v>
@@ -43710,7 +43726,7 @@
     </row>
     <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B611" s="10" t="n">
         <v>1</v>
@@ -43781,7 +43797,7 @@
     </row>
     <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A612" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B612" s="10" t="n">
         <v>1</v>
@@ -43852,7 +43868,7 @@
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B613" s="10" t="n">
         <v>1</v>
@@ -43923,7 +43939,7 @@
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B614" s="10" t="n">
         <v>1</v>
@@ -43994,7 +44010,7 @@
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B615" s="10" t="n">
         <v>1</v>
@@ -44065,7 +44081,7 @@
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B616" s="10" t="n">
         <v>1</v>
@@ -44136,7 +44152,7 @@
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A617" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B617" s="10" t="n">
         <v>1</v>
@@ -44207,7 +44223,7 @@
     </row>
     <row r="618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A618" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B618" s="10" t="n">
         <v>1</v>
@@ -44278,7 +44294,7 @@
     </row>
     <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B619" s="10" t="n">
         <v>1</v>
@@ -44349,7 +44365,7 @@
     </row>
     <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B620" s="10" t="n">
         <v>1</v>
@@ -44420,7 +44436,7 @@
     </row>
     <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B621" s="10" t="n">
         <v>1</v>
@@ -44491,7 +44507,7 @@
     </row>
     <row r="622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B622" s="10" t="n">
         <v>1</v>
@@ -44562,7 +44578,7 @@
     </row>
     <row r="623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B623" s="10" t="n">
         <v>1</v>
@@ -44633,7 +44649,7 @@
     </row>
     <row r="624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B624" s="10" t="n">
         <v>1</v>
@@ -44704,7 +44720,7 @@
     </row>
     <row r="625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B625" s="10" t="n">
         <v>1</v>
@@ -44775,7 +44791,7 @@
     </row>
     <row r="626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B626" s="10" t="n">
         <v>1</v>
@@ -44846,7 +44862,7 @@
     </row>
     <row r="627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B627" s="10" t="n">
         <v>1</v>
@@ -44917,7 +44933,7 @@
     </row>
     <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B628" s="10" t="n">
         <v>1</v>
@@ -44988,7 +45004,7 @@
     </row>
     <row r="629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B629" s="10" t="n">
         <v>1</v>
@@ -45059,7 +45075,7 @@
     </row>
     <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B630" s="10" t="n">
         <v>1</v>
@@ -45130,7 +45146,7 @@
     </row>
     <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B631" s="10" t="n">
         <v>1</v>
@@ -45201,7 +45217,7 @@
     </row>
     <row r="632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B632" s="10" t="n">
         <v>1</v>
@@ -45272,7 +45288,7 @@
     </row>
     <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B633" s="10" t="n">
         <v>1</v>
@@ -45343,7 +45359,7 @@
     </row>
     <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B634" s="10" t="n">
         <v>1</v>
@@ -45414,7 +45430,7 @@
     </row>
     <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A635" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B635" s="10" t="n">
         <v>1</v>
@@ -45485,7 +45501,7 @@
     </row>
     <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B636" s="10" t="n">
         <v>1</v>
@@ -45556,7 +45572,7 @@
     </row>
     <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B637" s="10" t="n">
         <v>1</v>
@@ -45627,7 +45643,7 @@
     </row>
     <row r="638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A638" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B638" s="10" t="n">
         <v>1</v>
@@ -45698,7 +45714,7 @@
     </row>
     <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B639" s="10" t="n">
         <v>1</v>
@@ -45769,7 +45785,7 @@
     </row>
     <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A640" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B640" s="10" t="n">
         <v>1</v>
@@ -45840,7 +45856,7 @@
     </row>
     <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B641" s="10" t="n">
         <v>1</v>
@@ -45911,7 +45927,7 @@
     </row>
     <row r="642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B642" s="10" t="n">
         <v>1</v>
@@ -45982,7 +45998,7 @@
     </row>
     <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B643" s="10" t="n">
         <v>1</v>
@@ -46053,7 +46069,7 @@
     </row>
     <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B644" s="10" t="n">
         <v>1</v>
@@ -46124,7 +46140,7 @@
     </row>
     <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B645" s="10" t="n">
         <v>1</v>
@@ -46195,7 +46211,7 @@
     </row>
     <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B646" s="10" t="n">
         <v>1</v>
@@ -46266,7 +46282,7 @@
     </row>
     <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B647" s="10" t="n">
         <v>1</v>
@@ -46337,7 +46353,7 @@
     </row>
     <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B648" s="10" t="n">
         <v>1</v>
@@ -46408,7 +46424,7 @@
     </row>
     <row r="649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B649" s="10" t="n">
         <v>1</v>
@@ -46479,7 +46495,7 @@
     </row>
     <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B650" s="10" t="n">
         <v>1</v>
@@ -46550,7 +46566,7 @@
     </row>
     <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B651" s="10" t="n">
         <v>1</v>
@@ -46621,7 +46637,7 @@
     </row>
     <row r="652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B652" s="10" t="n">
         <v>1</v>
@@ -46692,7 +46708,7 @@
     </row>
     <row r="653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B653" s="10" t="n">
         <v>1</v>
@@ -46763,7 +46779,7 @@
     </row>
     <row r="654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B654" s="10" t="n">
         <v>1</v>
@@ -46834,7 +46850,7 @@
     </row>
     <row r="655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B655" s="10" t="n">
         <v>1</v>
@@ -46905,7 +46921,7 @@
     </row>
     <row r="656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B656" s="10" t="n">
         <v>1</v>
@@ -46976,7 +46992,7 @@
     </row>
     <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B657" s="10" t="n">
         <v>1</v>
@@ -47047,7 +47063,7 @@
     </row>
     <row r="658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B658" s="10" t="n">
         <v>1</v>
@@ -47118,7 +47134,7 @@
     </row>
     <row r="659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B659" s="10" t="n">
         <v>1</v>
@@ -47189,7 +47205,7 @@
     </row>
     <row r="660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B660" s="10" t="n">
         <v>1</v>
@@ -47260,7 +47276,7 @@
     </row>
     <row r="661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B661" s="10" t="n">
         <v>1</v>
@@ -47331,7 +47347,7 @@
     </row>
     <row r="662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B662" s="10" t="n">
         <v>1</v>
@@ -47402,7 +47418,7 @@
     </row>
     <row r="663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B663" s="10" t="n">
         <v>1</v>
@@ -47473,7 +47489,7 @@
     </row>
     <row r="664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B664" s="10" t="n">
         <v>1</v>
@@ -47544,7 +47560,7 @@
     </row>
     <row r="665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B665" s="10" t="n">
         <v>1</v>
@@ -47615,7 +47631,7 @@
     </row>
     <row r="666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B666" s="10" t="n">
         <v>1</v>
@@ -47686,7 +47702,7 @@
     </row>
     <row r="667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B667" s="10" t="n">
         <v>1</v>
@@ -47757,7 +47773,7 @@
     </row>
     <row r="668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B668" s="10" t="n">
         <v>1</v>
@@ -47828,7 +47844,7 @@
     </row>
     <row r="669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B669" s="10" t="n">
         <v>1</v>
@@ -47899,7 +47915,7 @@
     </row>
     <row r="670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B670" s="10" t="n">
         <v>1</v>
@@ -47970,7 +47986,7 @@
     </row>
     <row r="671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B671" s="10" t="n">
         <v>1</v>
@@ -48041,7 +48057,7 @@
     </row>
     <row r="672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B672" s="10" t="n">
         <v>1</v>
@@ -48112,7 +48128,7 @@
     </row>
     <row r="673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B673" s="10" t="n">
         <v>1</v>
@@ -48183,7 +48199,7 @@
     </row>
     <row r="674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B674" s="10" t="n">
         <v>1</v>
@@ -48254,7 +48270,7 @@
     </row>
     <row r="675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B675" s="10" t="n">
         <v>1</v>
@@ -48325,7 +48341,7 @@
     </row>
     <row r="676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B676" s="10" t="n">
         <v>1</v>
@@ -48396,7 +48412,7 @@
     </row>
     <row r="677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B677" s="10" t="n">
         <v>1</v>
@@ -48467,7 +48483,7 @@
     </row>
     <row r="678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B678" s="10" t="n">
         <v>1</v>
@@ -48538,7 +48554,7 @@
     </row>
     <row r="679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B679" s="10" t="n">
         <v>1</v>
@@ -48609,7 +48625,7 @@
     </row>
     <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B680" s="10" t="n">
         <v>1</v>
@@ -48680,7 +48696,7 @@
     </row>
     <row r="681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B681" s="10" t="n">
         <v>1</v>
@@ -48751,7 +48767,7 @@
     </row>
     <row r="682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B682" s="10" t="n">
         <v>1</v>
@@ -48822,7 +48838,7 @@
     </row>
     <row r="683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B683" s="10" t="n">
         <v>1</v>
@@ -48893,7 +48909,7 @@
     </row>
     <row r="684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B684" s="10" t="n">
         <v>1</v>
@@ -48964,7 +48980,7 @@
     </row>
     <row r="685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B685" s="10" t="n">
         <v>1</v>
@@ -49035,7 +49051,7 @@
     </row>
     <row r="686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B686" s="10" t="n">
         <v>1</v>
@@ -49106,7 +49122,7 @@
     </row>
     <row r="687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B687" s="10" t="n">
         <v>1</v>
@@ -49177,7 +49193,7 @@
     </row>
     <row r="688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B688" s="10" t="n">
         <v>1</v>
@@ -49248,7 +49264,7 @@
     </row>
     <row r="689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A689" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B689" s="10" t="n">
         <v>1</v>
@@ -49319,7 +49335,7 @@
     </row>
     <row r="690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B690" s="10" t="n">
         <v>1</v>
@@ -49390,7 +49406,7 @@
     </row>
     <row r="691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A691" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B691" s="10" t="n">
         <v>1</v>
@@ -49461,7 +49477,7 @@
     </row>
     <row r="692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A692" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B692" s="10" t="n">
         <v>1</v>
@@ -49532,7 +49548,7 @@
     </row>
     <row r="693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B693" s="10" t="n">
         <v>1</v>
@@ -49603,7 +49619,7 @@
     </row>
     <row r="694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A694" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B694" s="10" t="n">
         <v>1</v>
@@ -49674,7 +49690,7 @@
     </row>
     <row r="695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B695" s="10" t="n">
         <v>1</v>
@@ -49745,7 +49761,7 @@
     </row>
     <row r="696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B696" s="10" t="n">
         <v>1</v>
@@ -49816,7 +49832,7 @@
     </row>
     <row r="697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A697" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B697" s="10" t="n">
         <v>1</v>
@@ -49887,7 +49903,7 @@
     </row>
     <row r="698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A698" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B698" s="10" t="n">
         <v>1</v>
@@ -49958,7 +49974,7 @@
     </row>
     <row r="699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A699" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B699" s="10" t="n">
         <v>1</v>
@@ -50029,7 +50045,7 @@
     </row>
     <row r="700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A700" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B700" s="10" t="n">
         <v>1</v>
@@ -50100,7 +50116,7 @@
     </row>
     <row r="701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A701" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B701" s="10" t="n">
         <v>1</v>
@@ -50171,7 +50187,7 @@
     </row>
     <row r="702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A702" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B702" s="10" t="n">
         <v>1</v>
@@ -50242,7 +50258,7 @@
     </row>
     <row r="703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A703" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B703" s="10" t="n">
         <v>1</v>
@@ -50313,7 +50329,7 @@
     </row>
     <row r="704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A704" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B704" s="10" t="n">
         <v>1</v>
@@ -50384,7 +50400,7 @@
     </row>
     <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B705" s="10" t="n">
         <v>1</v>
@@ -50455,7 +50471,7 @@
     </row>
     <row r="706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A706" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B706" s="10" t="n">
         <v>1</v>
@@ -50526,7 +50542,7 @@
     </row>
     <row r="707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A707" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B707" s="10" t="n">
         <v>1</v>
@@ -50597,7 +50613,7 @@
     </row>
     <row r="708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A708" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B708" s="10" t="n">
         <v>1</v>
@@ -50668,7 +50684,7 @@
     </row>
     <row r="709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A709" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B709" s="10" t="n">
         <v>1</v>
@@ -50739,7 +50755,7 @@
     </row>
     <row r="710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A710" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B710" s="10" t="n">
         <v>1</v>
@@ -50810,7 +50826,7 @@
     </row>
     <row r="711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A711" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B711" s="10" t="n">
         <v>1</v>
@@ -50881,7 +50897,7 @@
     </row>
     <row r="712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A712" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B712" s="10" t="n">
         <v>1</v>
@@ -50952,7 +50968,7 @@
     </row>
     <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B713" s="10" t="n">
         <v>1</v>
@@ -51023,7 +51039,7 @@
     </row>
     <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A714" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B714" s="10" t="n">
         <v>1</v>
@@ -51094,7 +51110,7 @@
     </row>
     <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A715" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B715" s="10" t="n">
         <v>1</v>
@@ -51165,7 +51181,7 @@
     </row>
     <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A716" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B716" s="10" t="n">
         <v>1</v>
@@ -51236,7 +51252,7 @@
     </row>
     <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A717" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B717" s="10" t="n">
         <v>1</v>
@@ -51307,7 +51323,7 @@
     </row>
     <row r="718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A718" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B718" s="10" t="n">
         <v>1</v>
@@ -51378,7 +51394,7 @@
     </row>
     <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A719" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B719" s="10" t="n">
         <v>1</v>
@@ -51449,7 +51465,7 @@
     </row>
     <row r="720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A720" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B720" s="10" t="n">
         <v>1</v>
@@ -51520,7 +51536,7 @@
     </row>
     <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A721" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B721" s="10" t="n">
         <v>1</v>
@@ -51591,7 +51607,7 @@
     </row>
     <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A722" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B722" s="10" t="n">
         <v>1</v>
@@ -51662,7 +51678,7 @@
     </row>
     <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A723" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B723" s="10" t="n">
         <v>1</v>
@@ -51733,7 +51749,7 @@
     </row>
     <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B724" s="10" t="n">
         <v>1</v>
@@ -51804,7 +51820,7 @@
     </row>
     <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A725" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B725" s="10" t="n">
         <v>1</v>
@@ -51875,7 +51891,7 @@
     </row>
     <row r="726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A726" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B726" s="10" t="n">
         <v>1</v>
@@ -51946,7 +51962,7 @@
     </row>
     <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A727" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B727" s="10" t="n">
         <v>1</v>
@@ -52017,7 +52033,7 @@
     </row>
     <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A728" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B728" s="10" t="n">
         <v>1</v>
@@ -52088,7 +52104,7 @@
     </row>
     <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A729" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B729" s="10" t="n">
         <v>1</v>
@@ -52159,7 +52175,7 @@
     </row>
     <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A730" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B730" s="10" t="n">
         <v>1</v>
@@ -52230,7 +52246,7 @@
     </row>
     <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A731" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B731" s="10" t="n">
         <v>1</v>
@@ -52301,7 +52317,7 @@
     </row>
     <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A732" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B732" s="10" t="n">
         <v>1</v>
@@ -52372,7 +52388,7 @@
     </row>
     <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A733" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B733" s="10" t="n">
         <v>1</v>
@@ -52443,7 +52459,7 @@
     </row>
     <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A734" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B734" s="10" t="n">
         <v>1</v>
@@ -52514,7 +52530,7 @@
     </row>
     <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A735" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B735" s="10" t="n">
         <v>1</v>
@@ -52585,7 +52601,7 @@
     </row>
     <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B736" s="10" t="n">
         <v>1</v>
@@ -52656,7 +52672,7 @@
     </row>
     <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A737" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B737" s="10" t="n">
         <v>1</v>
@@ -52727,7 +52743,7 @@
     </row>
     <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A738" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B738" s="10" t="n">
         <v>1</v>
@@ -52798,7 +52814,7 @@
     </row>
     <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A739" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B739" s="10" t="n">
         <v>1</v>
@@ -52869,7 +52885,7 @@
     </row>
     <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A740" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B740" s="10" t="n">
         <v>1</v>
@@ -52940,7 +52956,7 @@
     </row>
     <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A741" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B741" s="10" t="n">
         <v>1</v>
@@ -53011,7 +53027,7 @@
     </row>
     <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A742" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B742" s="10" t="n">
         <v>1</v>
@@ -53082,7 +53098,7 @@
     </row>
     <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A743" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B743" s="10" t="n">
         <v>1</v>
@@ -53153,7 +53169,7 @@
     </row>
     <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A744" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B744" s="10" t="n">
         <v>1</v>
@@ -53224,7 +53240,7 @@
     </row>
     <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A745" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B745" s="10" t="n">
         <v>1</v>
@@ -53242,7 +53258,7 @@
         <v>2.87785277394444</v>
       </c>
       <c r="G745" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H745" s="10" t="n">
         <v>5.80516103406667</v>
@@ -53295,7 +53311,7 @@
     </row>
     <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A746" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B746" s="10" t="n">
         <v>1</v>
@@ -53366,7 +53382,7 @@
     </row>
     <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A747" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B747" s="10" t="n">
         <v>1</v>
@@ -53437,7 +53453,7 @@
     </row>
     <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A748" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B748" s="10" t="n">
         <v>1</v>
@@ -53508,7 +53524,7 @@
     </row>
     <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A749" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B749" s="10" t="n">
         <v>1</v>
@@ -53579,7 +53595,7 @@
     </row>
     <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A750" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B750" s="10" t="n">
         <v>1</v>
@@ -53650,7 +53666,7 @@
     </row>
     <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A751" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B751" s="10" t="n">
         <v>1</v>
@@ -53721,7 +53737,7 @@
     </row>
     <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A752" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B752" s="10" t="n">
         <v>1</v>
@@ -53792,7 +53808,7 @@
     </row>
     <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A753" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B753" s="10" t="n">
         <v>1</v>
@@ -53863,7 +53879,7 @@
     </row>
     <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A754" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B754" s="10" t="n">
         <v>1</v>
@@ -53934,7 +53950,7 @@
     </row>
     <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A755" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B755" s="10" t="n">
         <v>1</v>
@@ -54005,7 +54021,7 @@
     </row>
     <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A756" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B756" s="10" t="n">
         <v>1</v>
@@ -54076,7 +54092,7 @@
     </row>
     <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A757" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B757" s="10" t="n">
         <v>1</v>
@@ -54147,7 +54163,7 @@
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A758" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B758" s="10" t="n">
         <v>1</v>
@@ -54218,7 +54234,7 @@
     </row>
     <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A759" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B759" s="10" t="n">
         <v>1</v>
@@ -54289,7 +54305,7 @@
     </row>
     <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A760" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B760" s="10" t="n">
         <v>1</v>
@@ -54360,7 +54376,7 @@
     </row>
     <row r="761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A761" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B761" s="10" t="n">
         <v>1</v>
@@ -54431,7 +54447,7 @@
     </row>
     <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A762" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B762" s="10" t="n">
         <v>1</v>
@@ -54502,7 +54518,7 @@
     </row>
     <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A763" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B763" s="10" t="n">
         <v>1</v>
@@ -54573,7 +54589,7 @@
     </row>
     <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A764" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B764" s="10" t="n">
         <v>1</v>
@@ -54644,7 +54660,7 @@
     </row>
     <row r="765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A765" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B765" s="10" t="n">
         <v>1</v>
@@ -54715,7 +54731,7 @@
     </row>
     <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A766" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B766" s="10" t="n">
         <v>1</v>
@@ -54786,7 +54802,7 @@
     </row>
     <row r="767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A767" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B767" s="10" t="n">
         <v>1</v>
@@ -54979,7 +54995,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -54996,7 +55012,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -55013,7 +55029,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -55030,7 +55046,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
mostly done the R section
</commit_message>
<xml_diff>
--- a/R/data_files/snark.measures.xlsx
+++ b/R/data_files/snark.measures.xlsx
@@ -114,7 +114,7 @@
     <t>standard deviation</t>
   </si>
   <si>
-    <t>Addis</t>
+    <t>Juneau</t>
   </si>
   <si>
     <t>NA</t>
@@ -129,7 +129,7 @@
     <t>6.01613987474441*</t>
   </si>
   <si>
-    <t>Juneau</t>
+    <t>Addis</t>
   </si>
   <si>
     <t>388.26000185323*</t>
@@ -422,8 +422,8 @@
       <c:layout/>
     </c:title>
     <c:view3D>
-      <c:rotX val="17"/>
-      <c:rotY val="20"/>
+      <c:rotX val="18"/>
+      <c:rotY val="19"/>
       <c:rAngAx val="1"/>
       <c:perspective val="40"/>
     </c:view3D>
@@ -562,14 +562,24 @@
             </a:ln>
           </c:spPr>
         </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="cylinder"/>
-        <c:axId val="13863742"/>
-        <c:axId val="46439789"/>
+        <c:axId val="45663193"/>
+        <c:axId val="49562736"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="13863742"/>
+        <c:axId val="45663193"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,14 +595,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46439789"/>
+        <c:crossAx val="49562736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46439789"/>
+        <c:axId val="49562736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +627,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13863742"/>
+        <c:crossAx val="45663193"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -657,15 +667,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>208440</xdr:colOff>
+      <xdr:colOff>235440</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>276480</xdr:colOff>
+      <xdr:colOff>303120</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>131040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -673,8 +683,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5897880" y="1129320"/>
-        <a:ext cx="5757480" cy="3237480"/>
+        <a:off x="5924880" y="1120320"/>
+        <a:ext cx="5757120" cy="3237120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -694,8 +704,8 @@
   </sheetPr>
   <dimension ref="A1:AC982"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N541" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O556" activeCellId="0" sqref="O556"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -900,7 +910,7 @@
       <c r="X8" s="0"/>
       <c r="Y8" s="4" t="str">
         <f aca="false">A8</f>
-        <v>Addis</v>
+        <v>Juneau</v>
       </c>
       <c r="Z8" s="4" t="n">
         <f aca="false">B8</f>
@@ -11216,7 +11226,7 @@
       <c r="X153" s="0"/>
       <c r="Y153" s="5" t="str">
         <f aca="false">A153</f>
-        <v>Addis</v>
+        <v>Juneau</v>
       </c>
       <c r="Z153" s="5" t="n">
         <f aca="false">B153</f>
@@ -22881,7 +22891,7 @@
       <c r="X317" s="0"/>
       <c r="Y317" s="8" t="str">
         <f aca="false">A317</f>
-        <v>Juneau</v>
+        <v>Addis</v>
       </c>
       <c r="Z317" s="8" t="n">
         <f aca="false">B317</f>
@@ -38664,7 +38674,7 @@
       <c r="X539" s="0"/>
       <c r="Y539" s="9" t="str">
         <f aca="false">A539</f>
-        <v>Juneau</v>
+        <v>Addis</v>
       </c>
       <c r="Z539" s="9" t="n">
         <f aca="false">B539</f>
@@ -54961,7 +54971,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -54978,7 +54988,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -54995,7 +55005,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -55012,7 +55022,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>

</xml_diff>